<commit_message>
Test specs for Inloggningsfunktion and Integrationstester has been updated.
</commit_message>
<xml_diff>
--- a/Del_1-Rapport/Test_Specifikation_Integrationstester.xlsx
+++ b/Del_1-Rapport/Test_Specifikation_Integrationstester.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studies\Testautomation_CI_CD\InlämningsUppgift_TA\Del_1-Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BD1C3F-7432-42EA-93EC-A324F792BA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476048FF-47E7-4795-A814-85AFBC06BC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
   </bookViews>
@@ -38,28 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
-    <t xml:space="preserve">Test case ID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test case name </t>
-  </si>
-  <si>
-    <t>Test case description</t>
-  </si>
-  <si>
     <t>Req ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected result </t>
-  </si>
-  <si>
-    <t>Actual result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verdict </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Environment </t>
   </si>
   <si>
     <t>OS</t>
@@ -139,9 +118,6 @@
   </si>
   <si>
     <t>#4</t>
-  </si>
-  <si>
-    <t>Test specification- integrationstester</t>
   </si>
   <si>
     <t>def test_get_products_returns_200():</t>
@@ -272,10 +248,34 @@
     <t>Failed</t>
   </si>
   <si>
-    <t xml:space="preserve">Logs </t>
-  </si>
-  <si>
     <t>API:et returnerar statuskod 403. GitHub Actions saknar behörighet att få åtkomst till detta API.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Miljö </t>
+  </si>
+  <si>
+    <t>Test specifikation &amp; Resultat- Integrationstester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testfall ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testfall namn </t>
+  </si>
+  <si>
+    <t>Testfall beskrivning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Förväntade resultat </t>
+  </si>
+  <si>
+    <t>Faktiskt resultat</t>
+  </si>
+  <si>
+    <t>Dom</t>
+  </si>
+  <si>
+    <t>Loggar</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -483,28 +483,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -513,46 +539,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -892,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BBF6A0-D8E2-406A-AD12-25A43EEED0E6}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,539 +903,539 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+    </row>
+    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="28"/>
+    </row>
+    <row r="4" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="23"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="21"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="21"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-    </row>
-    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="E15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I15" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="19"/>
-    </row>
-    <row r="5" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-    </row>
-    <row r="9" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="24" t="s">
+      <c r="J15" s="23"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="22"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="24" t="s">
+      <c r="F17" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="H17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="E19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="24" t="s">
+      <c r="F21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="25" t="s">
+      <c r="G21" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="27"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="24" t="s">
+      <c r="H21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="24"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E23" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="32"/>
+    </row>
+    <row r="25" spans="1:11" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F25" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G25" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="31"/>
-      <c r="K19" s="22"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-    </row>
-    <row r="21" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="33"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-    </row>
-    <row r="23" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="24" t="s">
+      <c r="H25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="J23" s="31"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="1:11" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="I25" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="J25" s="31"/>
+      <c r="J25" s="17"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D22:K22"/>
+    <mergeCell ref="D24:K24"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="D14:K14"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="D20:K20"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="D8:K8"/>
-    <mergeCell ref="D10:K10"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="D14:K14"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="D18:K18"/>
-    <mergeCell ref="D20:K20"/>
-    <mergeCell ref="D22:K22"/>
-    <mergeCell ref="D24:K24"/>
-    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="I6:J6"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="A7:B26"/>
     <mergeCell ref="C7:C26"/>
@@ -1453,9 +1446,9 @@
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D10:K10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1" xr:uid="{26C8995E-A49B-4F9C-9D12-A335DDD70388}"/>

</xml_diff>